<commit_message>
Added FileManager for xlsx files
</commit_message>
<xml_diff>
--- a/calorie-count/Calorie_Counting.xlsx
+++ b/calorie-count/Calorie_Counting.xlsx
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -560,6 +560,316 @@
       </c>
       <c r="I4" t="n">
         <v>136.44</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>dsasdds</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>91.033</v>
+      </c>
+      <c r="C5" t="n">
+        <v>25</v>
+      </c>
+      <c r="D5" t="n">
+        <v>33</v>
+      </c>
+      <c r="E5" t="n">
+        <v>33</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>33</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>54345</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>91.033</v>
+      </c>
+      <c r="C6" t="n">
+        <v>25</v>
+      </c>
+      <c r="D6" t="n">
+        <v>33</v>
+      </c>
+      <c r="E6" t="n">
+        <v>33</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>33</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>dfdsf</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>91.033</v>
+      </c>
+      <c r="C7" t="n">
+        <v>25</v>
+      </c>
+      <c r="D7" t="n">
+        <v>33</v>
+      </c>
+      <c r="E7" t="n">
+        <v>33</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>33</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>987gg</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>91.033</v>
+      </c>
+      <c r="C8" t="n">
+        <v>25</v>
+      </c>
+      <c r="D8" t="n">
+        <v>33</v>
+      </c>
+      <c r="E8" t="n">
+        <v>33</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>33</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>aaaa</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>91.033</v>
+      </c>
+      <c r="C9" t="n">
+        <v>25</v>
+      </c>
+      <c r="D9" t="n">
+        <v>33</v>
+      </c>
+      <c r="E9" t="n">
+        <v>33</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>33</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>bbbb</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>91.033</v>
+      </c>
+      <c r="C10" t="n">
+        <v>25</v>
+      </c>
+      <c r="D10" t="n">
+        <v>33</v>
+      </c>
+      <c r="E10" t="n">
+        <v>33</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>33</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>ccc</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>91.033</v>
+      </c>
+      <c r="C11" t="n">
+        <v>25</v>
+      </c>
+      <c r="D11" t="n">
+        <v>33</v>
+      </c>
+      <c r="E11" t="n">
+        <v>33</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>33</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>ddd</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>91.033</v>
+      </c>
+      <c r="C12" t="n">
+        <v>25</v>
+      </c>
+      <c r="D12" t="n">
+        <v>33</v>
+      </c>
+      <c r="E12" t="n">
+        <v>33</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>33</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>eeeee</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>91.033</v>
+      </c>
+      <c r="C13" t="n">
+        <v>25</v>
+      </c>
+      <c r="D13" t="n">
+        <v>33</v>
+      </c>
+      <c r="E13" t="n">
+        <v>33</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>33</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" t="n">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>fffs</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>91.033</v>
+      </c>
+      <c r="C14" t="n">
+        <v>25</v>
+      </c>
+      <c r="D14" t="n">
+        <v>33</v>
+      </c>
+      <c r="E14" t="n">
+        <v>33</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>33</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>529</v>
       </c>
     </row>
   </sheetData>
@@ -573,7 +883,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -713,6 +1023,69 @@
         <v>0.2</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2022-11-17</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Sherbet</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>98.760046</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1.16</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2022-11-17</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Sherbet</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>98.760046</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1.16</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2022-11-17</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>987gg</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>91.033</v>
+      </c>
+      <c r="D9" t="n">
+        <v>25</v>
+      </c>
+      <c r="E9" t="n">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>